<commit_message>
Updated the CSV files. - Matthew
</commit_message>
<xml_diff>
--- a/SQLFiles/Stuff.xlsx
+++ b/SQLFiles/Stuff.xlsx
@@ -5,18 +5,18 @@
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Project_Tracker\psychic-computing-machine\SQLFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\project_tracker\psychic-computing-machine\SQLFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Email" sheetId="8" r:id="rId2"/>
     <sheet name="Project" sheetId="5" r:id="rId3"/>
     <sheet name="Office" sheetId="7" r:id="rId4"/>
-    <sheet name="Phone" sheetId="6" r:id="rId5"/>
+    <sheet name="Phone02" sheetId="6" r:id="rId5"/>
     <sheet name="User" sheetId="4" r:id="rId6"/>
     <sheet name="UserData" sheetId="2" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId8"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="857" uniqueCount="430">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="872" uniqueCount="438">
   <si>
     <t>username</t>
   </si>
@@ -1242,9 +1242,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>NSA</t>
   </si>
   <si>
@@ -1324,6 +1321,33 @@
   </si>
   <si>
     <t>School</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>FinalDefenseDate</t>
+  </si>
+  <si>
+    <t>PlagiarismPercentage</t>
+  </si>
+  <si>
+    <t>ProjectGrade</t>
+  </si>
+  <si>
+    <t>CommitteeID</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -3726,7 +3750,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -3742,10 +3766,10 @@
         <v>393</v>
       </c>
       <c r="B1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" t="s">
         <v>427</v>
-      </c>
-      <c r="C1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3758,7 +3782,7 @@
         <v>ab1234@rit.edu</v>
       </c>
       <c r="C2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3771,7 +3795,7 @@
         <v>dn1234@rit.edu</v>
       </c>
       <c r="C3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3784,7 +3808,7 @@
         <v>gs1234@rit.edu</v>
       </c>
       <c r="C4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,7 +3821,7 @@
         <v>txaics@rit.edu</v>
       </c>
       <c r="C5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3810,7 +3834,7 @@
         <v>gpavks@rit.edu</v>
       </c>
       <c r="C6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3823,7 +3847,7 @@
         <v>daniel.ashbrook@rit.edu</v>
       </c>
       <c r="C7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3836,7 +3860,7 @@
         <v>catherine.beaton@rit.edu</v>
       </c>
       <c r="C8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3849,7 +3873,7 @@
         <v>aobics@rit.edu</v>
       </c>
       <c r="C9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3862,7 +3886,7 @@
         <v>tsbics@rit.edu</v>
       </c>
       <c r="C10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3875,7 +3899,7 @@
         <v>dsbics@rit.edu</v>
       </c>
       <c r="C11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3888,7 +3912,7 @@
         <v>cbbics@rit.edu</v>
       </c>
       <c r="C12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3901,7 +3925,7 @@
         <v>Sean.Boyle@rit.edu</v>
       </c>
       <c r="C13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3914,7 +3938,7 @@
         <v>mjcics@rit.edu</v>
       </c>
       <c r="C14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3927,7 +3951,7 @@
         <v>mjcvks@rit.edu</v>
       </c>
       <c r="C15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3940,7 +3964,7 @@
         <v>Michael.Floeser@rit.edu</v>
       </c>
       <c r="C16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3953,7 +3977,7 @@
         <v>nick@saunders.rit.edu</v>
       </c>
       <c r="C17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3966,7 +3990,7 @@
         <v>bdfvks@rit.edu</v>
       </c>
       <c r="C18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3979,7 +4003,7 @@
         <v>Dean.Ganskop@rit.edu</v>
       </c>
       <c r="C19" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3992,7 +4016,7 @@
         <v>efgics@rit.edu</v>
       </c>
       <c r="C20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4005,7 +4029,7 @@
         <v>jrhicsa@rit.edu</v>
       </c>
       <c r="C21" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4018,7 +4042,7 @@
         <v>vlh@rit.edu</v>
       </c>
       <c r="C22" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4031,7 +4055,7 @@
         <v>Bruce.Hartpence@rit.edu</v>
       </c>
       <c r="C23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4044,7 +4068,7 @@
         <v>amhgss@rit.edu</v>
       </c>
       <c r="C24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4057,7 +4081,7 @@
         <v>Lawrence.Hill@rit.edu</v>
       </c>
       <c r="C25" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4070,7 +4094,7 @@
         <v>edward.holden@rit.edu</v>
       </c>
       <c r="C26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4083,7 +4107,7 @@
         <v>matt.huenerfauth@rit.edu</v>
       </c>
       <c r="C27" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -4096,7 +4120,7 @@
         <v>jcjics@rit.edu</v>
       </c>
       <c r="C28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -4109,7 +4133,7 @@
         <v>mrjics@rit.edu</v>
       </c>
       <c r="C29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -4122,7 +4146,7 @@
         <v>jai.kang@rit.edu</v>
       </c>
       <c r="C30" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4135,7 +4159,7 @@
         <v>drkisd@rit.edu</v>
       </c>
       <c r="C31" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -4148,7 +4172,7 @@
         <v>hnkics@rit.edu</v>
       </c>
       <c r="C32" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4161,7 +4185,7 @@
         <v>mxkics1@rit.edu</v>
       </c>
       <c r="C33" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -4174,7 +4198,7 @@
         <v>dmlics@rit.edu</v>
       </c>
       <c r="C34" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4187,7 +4211,7 @@
         <v>Jeffrey.Lasky@rit.edu</v>
       </c>
       <c r="C35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4200,7 +4224,7 @@
         <v>jalvks@rit.edu</v>
       </c>
       <c r="C36" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4213,7 +4237,7 @@
         <v>jxlics@rit.edu</v>
       </c>
       <c r="C37" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4226,7 +4250,7 @@
         <v>Peter.Lutz@rit.edu</v>
       </c>
       <c r="C38" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4239,7 +4263,7 @@
         <v>Sharon.Mason@rit.edu</v>
       </c>
       <c r="C39" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4252,7 +4276,7 @@
         <v>mickmcquaid@gmail.com</v>
       </c>
       <c r="C40" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4265,7 +4289,7 @@
         <v>Tom.Oh@rit.edu</v>
       </c>
       <c r="C41" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4278,7 +4302,7 @@
         <v>sylvia.perez-hardy@rit.edu</v>
       </c>
       <c r="C42" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4291,7 +4315,7 @@
         <v>djpihst@rit.edu</v>
       </c>
       <c r="C43" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4304,7 +4328,7 @@
         <v>sarics@rit.edu</v>
       </c>
       <c r="C44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4317,7 +4341,7 @@
         <v>ldrics@rit.edu</v>
       </c>
       <c r="C45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4330,7 +4354,7 @@
         <v>kmsics@rit.edu</v>
       </c>
       <c r="C46" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4343,7 +4367,7 @@
         <v>cxsics@rit.edu</v>
       </c>
       <c r="C47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4356,7 +4380,7 @@
         <v>nxsvks@rit.edu</v>
       </c>
       <c r="C48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4369,7 +4393,7 @@
         <v>adam.smith@rit.edu</v>
       </c>
       <c r="C49" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4382,7 +4406,7 @@
         <v>jxtadm@rit.edu</v>
       </c>
       <c r="C50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4395,7 +4419,7 @@
         <v>bmtski@rit.edu</v>
       </c>
       <c r="C51" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4408,7 +4432,7 @@
         <v>rpv@mail.rit.edu</v>
       </c>
       <c r="C52" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4421,7 +4445,7 @@
         <v>axgvks@rit.edu</v>
       </c>
       <c r="C53" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4434,7 +4458,7 @@
         <v>emwics@rit.edu</v>
       </c>
       <c r="C54" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4447,7 +4471,7 @@
         <v>jswics@rit.edu</v>
       </c>
       <c r="C55" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -4460,7 +4484,7 @@
         <v>mayici@rit.edu</v>
       </c>
       <c r="C56" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4473,7 +4497,7 @@
         <v>qyuvks@rit.edu</v>
       </c>
       <c r="C57" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4486,7 +4510,7 @@
         <v>sjzics@rit.edu</v>
       </c>
       <c r="C58" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -4499,7 +4523,7 @@
         <v>rdbcst@rit.edu</v>
       </c>
       <c r="C59" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4512,7 +4536,7 @@
         <v>qyuvks@rit.edu</v>
       </c>
       <c r="C60" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -4522,10 +4546,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4537,46 +4561,70 @@
     <col min="6" max="8" width="9.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" t="s">
         <v>412</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>413</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>414</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>415</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>416</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>417</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>418</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>419</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>420</v>
       </c>
-      <c r="J1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>419</v>
+      </c>
+      <c r="L1" t="s">
+        <v>420</v>
+      </c>
+      <c r="M1" t="s">
+        <v>431</v>
+      </c>
+      <c r="N1" t="s">
+        <v>432</v>
+      </c>
+      <c r="O1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C2" t="str">
         <f>Users!M2</f>
@@ -4587,7 +4635,7 @@
         <v xml:space="preserve">Network implosion </v>
       </c>
       <c r="E2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F2" s="2" t="d">
         <v>2016-08-20</v>
@@ -4604,13 +4652,28 @@
       <c r="J2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>435</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C3" t="str">
         <f>Users!M3</f>
@@ -4621,7 +4684,7 @@
         <v>Program better with a beard</v>
       </c>
       <c r="E3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F3" s="2" t="d">
         <v>2016-08-16</v>
@@ -4638,13 +4701,28 @@
       <c r="J3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>436</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C4" t="str">
         <f>Users!M4</f>
@@ -4655,7 +4733,7 @@
         <v>Capstone tracking database</v>
       </c>
       <c r="E4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F4" s="2" t="d">
         <v>2015-08-14</v>
@@ -4671,6 +4749,21 @@
       </c>
       <c r="J4" t="b">
         <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>437</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4698,10 +4791,10 @@
         <v>393</v>
       </c>
       <c r="B1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1" t="s">
         <v>409</v>
-      </c>
-      <c r="C1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4738,7 +4831,7 @@
         <v>GOL 2315</v>
       </c>
       <c r="C6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4751,7 +4844,7 @@
         <v>GOL 2329</v>
       </c>
       <c r="C7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4764,7 +4857,7 @@
         <v>GOL 2621</v>
       </c>
       <c r="C8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4789,7 +4882,7 @@
         <v>GOL 2571</v>
       </c>
       <c r="C11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4802,7 +4895,7 @@
         <v>GOL 2615</v>
       </c>
       <c r="C12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4833,7 +4926,7 @@
         <v>GOL 2669</v>
       </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4945,7 @@
         <v>GOL 2619</v>
       </c>
       <c r="C18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4871,7 +4964,7 @@
         <v>GOL 2617</v>
       </c>
       <c r="C20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4890,7 +4983,7 @@
         <v>GOL 2645</v>
       </c>
       <c r="C22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4903,7 +4996,7 @@
         <v>GOL 2323</v>
       </c>
       <c r="C23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4916,7 +5009,7 @@
         <v>GOL 2323</v>
       </c>
       <c r="C24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4929,7 +5022,7 @@
         <v>GOL 2331</v>
       </c>
       <c r="C25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4942,7 +5035,7 @@
         <v>GOL 2655</v>
       </c>
       <c r="C26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4955,7 +5048,7 @@
         <v>GOL 2659</v>
       </c>
       <c r="C27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -4980,7 +5073,7 @@
         <v>GOL 2651</v>
       </c>
       <c r="C30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4993,7 +5086,7 @@
         <v>GOL 2285</v>
       </c>
       <c r="C31" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5018,7 +5111,7 @@
         <v>GOL 2627</v>
       </c>
       <c r="C34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5031,7 +5124,7 @@
         <v>GOL 26xx</v>
       </c>
       <c r="C35" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5044,7 +5137,7 @@
         <v>GOL 2657</v>
       </c>
       <c r="C36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5063,7 +5156,7 @@
         <v>GOL 2345</v>
       </c>
       <c r="C38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5076,7 +5169,7 @@
         <v>GOL 2319</v>
       </c>
       <c r="C39" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5095,7 +5188,7 @@
         <v>GOL 2281</v>
       </c>
       <c r="C41" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5114,7 +5207,7 @@
         <v>CBT-2161</v>
       </c>
       <c r="C43" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5169,7 +5262,7 @@
         <v>GOL 2673</v>
       </c>
       <c r="C51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5182,7 +5275,7 @@
         <v>GOL 2519</v>
       </c>
       <c r="C52" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5201,7 +5294,7 @@
         <v>GOL 2635</v>
       </c>
       <c r="C54" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5226,7 +5319,7 @@
         <v>GOL 2669</v>
       </c>
       <c r="C57" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5239,7 +5332,7 @@
         <v>GOL 2109</v>
       </c>
       <c r="C58" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5252,7 +5345,7 @@
         <v>GOL 2103</v>
       </c>
       <c r="C59" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5265,7 +5358,7 @@
         <v>GOL 2669</v>
       </c>
       <c r="C60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -5292,10 +5385,10 @@
         <v>393</v>
       </c>
       <c r="B1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1" t="s">
         <v>406</v>
-      </c>
-      <c r="C1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5332,7 +5425,7 @@
         <v>585-475-7854</v>
       </c>
       <c r="C6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5345,7 +5438,7 @@
         <v>585-475-4784</v>
       </c>
       <c r="C7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5358,7 +5451,7 @@
         <v>585-281-6162</v>
       </c>
       <c r="C8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5383,7 +5476,7 @@
         <v>585-4755231</v>
       </c>
       <c r="C11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5396,7 +5489,7 @@
         <v>585-475-7946</v>
       </c>
       <c r="C12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5427,7 +5520,7 @@
         <v>585-475-7031</v>
       </c>
       <c r="C16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5446,7 +5539,7 @@
         <v>585-475-6511</v>
       </c>
       <c r="C18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5477,7 +5570,7 @@
         <v>585-475-5384</v>
       </c>
       <c r="C22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5490,7 +5583,7 @@
         <v>585-475-7938</v>
       </c>
       <c r="C23" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5503,7 +5596,7 @@
         <v>585-475-4554</v>
       </c>
       <c r="C24" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5516,7 +5609,7 @@
         <v>585-475-7064</v>
       </c>
       <c r="C25" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5529,7 +5622,7 @@
         <v>585-475-5361</v>
       </c>
       <c r="C26" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5542,7 +5635,7 @@
         <v>585-475-2459</v>
       </c>
       <c r="C27" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5567,7 +5660,7 @@
         <v>585-475-5362</v>
       </c>
       <c r="C30" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5580,7 +5673,7 @@
         <v>585-475-2811</v>
       </c>
       <c r="C31" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5605,7 +5698,7 @@
         <v>585-475-5001</v>
       </c>
       <c r="C34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5618,7 +5711,7 @@
         <v>585-475-2284</v>
       </c>
       <c r="C35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5631,7 +5724,7 @@
         <v>585-475-6451</v>
       </c>
       <c r="C36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5650,7 +5743,7 @@
         <v>585-475-6162</v>
       </c>
       <c r="C38" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5663,7 +5756,7 @@
         <v>585-475-6989</v>
       </c>
       <c r="C39" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5682,7 +5775,7 @@
         <v>585-475-7642</v>
       </c>
       <c r="C41" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5695,7 +5788,7 @@
         <v>585-475-7941</v>
       </c>
       <c r="C42" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5708,7 +5801,7 @@
         <v>585-475-2487</v>
       </c>
       <c r="C43" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5751,7 +5844,7 @@
         <v>585-475-4552</v>
       </c>
       <c r="C49" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5770,7 +5863,7 @@
         <v>585-475-2869</v>
       </c>
       <c r="C51" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5783,7 +5876,7 @@
         <v>585-475-7281</v>
       </c>
       <c r="C52" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5802,7 +5895,7 @@
         <v>585-475-6733</v>
       </c>
       <c r="C54" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5827,7 +5920,7 @@
         <v>585-475-6929</v>
       </c>
       <c r="C57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5840,7 +5933,7 @@
         <v>585-475-7643</v>
       </c>
       <c r="C58" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5853,7 +5946,7 @@
         <v>585-475-7924</v>
       </c>
       <c r="C59" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5866,7 +5959,7 @@
         <v>585-475-6929</v>
       </c>
       <c r="C60" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -5879,7 +5972,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F5" sqref="F5:F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5937,13 +6030,8 @@
         <f>Users!C2</f>
         <v>Baker</v>
       </c>
-      <c r="D2" t="str">
-        <f>Users!E2</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E2" t="str">
-        <f>Users!F2</f>
-        <v>UNKNOWN</v>
+      <c r="D2" t="s">
+        <v>430</v>
       </c>
       <c r="F2" s="2" t="d">
         <v>2017-05-15</v>
@@ -5953,11 +6041,10 @@
         <v>Grad</v>
       </c>
       <c r="H2" t="s">
-        <v>403</v>
-      </c>
-      <c r="I2" t="str">
-        <f>Users!J2</f>
-        <v>Grad</v>
+        <v>402</v>
+      </c>
+      <c r="I2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5973,13 +6060,8 @@
         <f>Users!C3</f>
         <v>Novello</v>
       </c>
-      <c r="D3" t="str">
-        <f>Users!E3</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E3" t="str">
-        <f>Users!F3</f>
-        <v>UNKNOWN</v>
+      <c r="D3" t="s">
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="d">
         <v>2017-05-15</v>
@@ -5989,11 +6071,10 @@
         <v>Grad</v>
       </c>
       <c r="H3" t="s">
-        <v>404</v>
-      </c>
-      <c r="I3" t="str">
-        <f>Users!J3</f>
-        <v>Grad</v>
+        <v>403</v>
+      </c>
+      <c r="I3" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6009,13 +6090,8 @@
         <f>Users!C4</f>
         <v>Sarducci</v>
       </c>
-      <c r="D4" t="str">
-        <f>Users!E4</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E4" t="str">
-        <f>Users!F4</f>
-        <v>UNKNOWN</v>
+      <c r="D4" t="s">
+        <v>430</v>
       </c>
       <c r="F4" s="2" t="d">
         <v>2016-05-13</v>
@@ -6025,11 +6101,10 @@
         <v>Grad</v>
       </c>
       <c r="H4" t="s">
-        <v>405</v>
-      </c>
-      <c r="I4" t="str">
-        <f>Users!J4</f>
-        <v>Grad</v>
+        <v>404</v>
+      </c>
+      <c r="I4" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6045,16 +6120,8 @@
         <f>Users!C5</f>
         <v>Alam</v>
       </c>
-      <c r="D5" t="str">
-        <f>Users!E5</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E5">
-        <f>Users!F5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>402</v>
+      <c r="D5" t="s">
+        <v>430</v>
       </c>
       <c r="G5" t="str">
         <f>Users!J5</f>
@@ -6078,16 +6145,12 @@
         <f>Users!C6</f>
         <v>Arcoraci</v>
       </c>
-      <c r="D6" t="str">
-        <f>Users!E6</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D6" t="s">
+        <v>430</v>
       </c>
       <c r="E6" t="str">
         <f>Users!F6</f>
         <v>https://ist.rit.edu/assets/img/people/gpavks.jpg</v>
-      </c>
-      <c r="F6" t="s">
-        <v>402</v>
       </c>
       <c r="G6" t="str">
         <f>Users!J6</f>
@@ -6111,16 +6174,12 @@
         <f>Users!C7</f>
         <v>Ashbrook</v>
       </c>
-      <c r="D7" t="str">
-        <f>Users!E7</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D7" t="s">
+        <v>430</v>
       </c>
       <c r="E7" t="str">
         <f>Users!F7</f>
         <v>https://ist.rit.edu/assets/img/people/dlaics.jpg</v>
-      </c>
-      <c r="F7" t="s">
-        <v>402</v>
       </c>
       <c r="G7" t="str">
         <f>Users!J7</f>
@@ -6144,16 +6203,12 @@
         <f>Users!C8</f>
         <v>Beaton</v>
       </c>
-      <c r="D8" t="str">
-        <f>Users!E8</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D8" t="s">
+        <v>430</v>
       </c>
       <c r="E8" t="str">
         <f>Users!F8</f>
         <v>https://ist.rit.edu/assets/img/people/ciiics.jpg</v>
-      </c>
-      <c r="F8" t="s">
-        <v>402</v>
       </c>
       <c r="G8" t="str">
         <f>Users!J8</f>
@@ -6177,16 +6232,8 @@
         <f>Users!C9</f>
         <v>Berenbaum</v>
       </c>
-      <c r="D9" t="str">
-        <f>Users!E9</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E9">
-        <f>Users!F9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>402</v>
+      <c r="D9" t="s">
+        <v>430</v>
       </c>
       <c r="G9" t="str">
         <f>Users!J9</f>
@@ -6210,16 +6257,8 @@
         <f>Users!C10</f>
         <v>Bernhard</v>
       </c>
-      <c r="D10" t="str">
-        <f>Users!E10</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E10">
-        <f>Users!F10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>402</v>
+      <c r="D10" t="s">
+        <v>430</v>
       </c>
       <c r="G10" t="str">
         <f>Users!J10</f>
@@ -6243,16 +6282,12 @@
         <f>Users!C11</f>
         <v>Bogaard</v>
       </c>
-      <c r="D11" t="str">
-        <f>Users!E11</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D11" t="s">
+        <v>430</v>
       </c>
       <c r="E11" t="str">
         <f>Users!F11</f>
         <v>https://ist.rit.edu/assets/img/people/dsbics.jpg</v>
-      </c>
-      <c r="F11" t="s">
-        <v>402</v>
       </c>
       <c r="G11" t="str">
         <f>Users!J11</f>
@@ -6276,16 +6311,12 @@
         <f>Users!C12</f>
         <v>Border</v>
       </c>
-      <c r="D12" t="str">
-        <f>Users!E12</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D12" t="s">
+        <v>430</v>
       </c>
       <c r="E12" t="str">
         <f>Users!F12</f>
         <v>https://ist.rit.edu/assets/img/people/cbbics.jpg</v>
-      </c>
-      <c r="F12" t="s">
-        <v>402</v>
       </c>
       <c r="G12" t="str">
         <f>Users!J12</f>
@@ -6309,16 +6340,12 @@
         <f>Users!C13</f>
         <v>Boyle</v>
       </c>
-      <c r="D13" t="str">
-        <f>Users!E13</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D13" t="s">
+        <v>430</v>
       </c>
       <c r="E13" t="str">
         <f>Users!F13</f>
         <v>https://www.rit.edu/gccis/sites/rit.edu.gccis/files//Boyle%20Sean%20new%20headshot.jpg</v>
-      </c>
-      <c r="F13" t="s">
-        <v>402</v>
       </c>
       <c r="G13" t="str">
         <f>Users!J13</f>
@@ -6342,16 +6369,8 @@
         <f>Users!C14</f>
         <v>Carroll</v>
       </c>
-      <c r="D14" t="str">
-        <f>Users!E14</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E14">
-        <f>Users!F14</f>
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>402</v>
+      <c r="D14" t="s">
+        <v>430</v>
       </c>
       <c r="G14" t="str">
         <f>Users!J14</f>
@@ -6375,16 +6394,8 @@
         <f>Users!C15</f>
         <v>Casale</v>
       </c>
-      <c r="D15" t="str">
-        <f>Users!E15</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E15">
-        <f>Users!F15</f>
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>402</v>
+      <c r="D15" t="s">
+        <v>430</v>
       </c>
       <c r="G15" t="str">
         <f>Users!J15</f>
@@ -6408,16 +6419,12 @@
         <f>Users!C16</f>
         <v>Floeser</v>
       </c>
-      <c r="D16" t="str">
-        <f>Users!E16</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D16" t="s">
+        <v>430</v>
       </c>
       <c r="E16" t="str">
         <f>Users!F16</f>
         <v>https://ist.rit.edu/assets/img/people/mjfics.jpg</v>
-      </c>
-      <c r="F16" t="s">
-        <v>402</v>
       </c>
       <c r="G16" t="str">
         <f>Users!J16</f>
@@ -6441,16 +6448,8 @@
         <f>Users!C17</f>
         <v>Francesco</v>
       </c>
-      <c r="D17" t="str">
-        <f>Users!E17</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E17">
-        <f>Users!F17</f>
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>402</v>
+      <c r="D17" t="s">
+        <v>430</v>
       </c>
       <c r="G17" t="str">
         <f>Users!J17</f>
@@ -6474,16 +6473,12 @@
         <f>Users!C18</f>
         <v>French</v>
       </c>
-      <c r="D18" t="str">
-        <f>Users!E18</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D18" t="s">
+        <v>430</v>
       </c>
       <c r="E18" t="str">
         <f>Users!F18</f>
         <v>https://ist.rit.edu/assets/img/people/bdfvks.jpg</v>
-      </c>
-      <c r="F18" t="s">
-        <v>402</v>
       </c>
       <c r="G18" t="str">
         <f>Users!J18</f>
@@ -6507,16 +6502,8 @@
         <f>Users!C19</f>
         <v>Ganskop</v>
       </c>
-      <c r="D19" t="str">
-        <f>Users!E19</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E19">
-        <f>Users!F19</f>
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>402</v>
+      <c r="D19" t="s">
+        <v>430</v>
       </c>
       <c r="G19" t="str">
         <f>Users!J19</f>
@@ -6540,16 +6527,12 @@
         <f>Users!C20</f>
         <v>Golen</v>
       </c>
-      <c r="D20" t="str">
-        <f>Users!E20</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D20" t="s">
+        <v>430</v>
       </c>
       <c r="E20" t="str">
         <f>Users!F20</f>
         <v>https://ist.rit.edu/assets/img/people/efgics.jpg</v>
-      </c>
-      <c r="F20" t="s">
-        <v>402</v>
       </c>
       <c r="G20" t="str">
         <f>Users!J20</f>
@@ -6573,16 +6556,8 @@
         <f>Users!C21</f>
         <v>Habermas</v>
       </c>
-      <c r="D21" t="str">
-        <f>Users!E21</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E21">
-        <f>Users!F21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>402</v>
+      <c r="D21" t="s">
+        <v>430</v>
       </c>
       <c r="G21" t="str">
         <f>Users!J21</f>
@@ -6606,16 +6581,12 @@
         <f>Users!C22</f>
         <v>Hanson</v>
       </c>
-      <c r="D22" t="str">
-        <f>Users!E22</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D22" t="s">
+        <v>430</v>
       </c>
       <c r="E22" t="str">
         <f>Users!F22</f>
         <v>https://ist.rit.edu/assets/img/people/vlhics.jpg</v>
-      </c>
-      <c r="F22" t="s">
-        <v>402</v>
       </c>
       <c r="G22" t="str">
         <f>Users!J22</f>
@@ -6639,16 +6610,12 @@
         <f>Users!C23</f>
         <v>Hartpence</v>
       </c>
-      <c r="D23" t="str">
-        <f>Users!E23</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D23" t="s">
+        <v>430</v>
       </c>
       <c r="E23" t="str">
         <f>Users!F23</f>
         <v>https://ist.rit.edu/assets/img/people/bhhics.jpg</v>
-      </c>
-      <c r="F23" t="s">
-        <v>402</v>
       </c>
       <c r="G23" t="str">
         <f>Users!J23</f>
@@ -6672,16 +6639,12 @@
         <f>Users!C24</f>
         <v>Herbert</v>
       </c>
-      <c r="D24" t="str">
-        <f>Users!E24</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D24" t="s">
+        <v>430</v>
       </c>
       <c r="E24" t="str">
         <f>Users!F24</f>
         <v>https://ist.rit.edu/assets/img/people/amhgss.jpg</v>
-      </c>
-      <c r="F24" t="s">
-        <v>402</v>
       </c>
       <c r="G24" t="str">
         <f>Users!J24</f>
@@ -6705,16 +6668,12 @@
         <f>Users!C25</f>
         <v>Hill</v>
       </c>
-      <c r="D25" t="str">
-        <f>Users!E25</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D25" t="s">
+        <v>430</v>
       </c>
       <c r="E25" t="str">
         <f>Users!F25</f>
         <v>https://ist.rit.edu/assets/img/people/lwhfac.jpg</v>
-      </c>
-      <c r="F25" t="s">
-        <v>402</v>
       </c>
       <c r="G25" t="str">
         <f>Users!J25</f>
@@ -6738,16 +6697,12 @@
         <f>Users!C26</f>
         <v>Holden</v>
       </c>
-      <c r="D26" t="str">
-        <f>Users!E26</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D26" t="s">
+        <v>430</v>
       </c>
       <c r="E26" t="str">
         <f>Users!F26</f>
         <v>https://ist.rit.edu/assets/img/people/ephics.jpg</v>
-      </c>
-      <c r="F26" t="s">
-        <v>402</v>
       </c>
       <c r="G26" t="str">
         <f>Users!J26</f>
@@ -6771,16 +6726,12 @@
         <f>Users!C27</f>
         <v>Huenerfauth</v>
       </c>
-      <c r="D27" t="str">
-        <f>Users!E27</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D27" t="s">
+        <v>430</v>
       </c>
       <c r="E27" t="str">
         <f>Users!F27</f>
         <v>https://ist.rit.edu/assets/img/people/mphics.jpg</v>
-      </c>
-      <c r="F27" t="s">
-        <v>402</v>
       </c>
       <c r="G27" t="str">
         <f>Users!J27</f>
@@ -6804,16 +6755,12 @@
         <f>Users!C28</f>
         <v>Jockel</v>
       </c>
-      <c r="D28" t="str">
-        <f>Users!E28</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D28" t="s">
+        <v>430</v>
       </c>
       <c r="E28" t="str">
         <f>Users!F28</f>
         <v>https://www.rit.edu/gccis/sites/rit.edu.gccis/files//Jeff%20IST%20small.jpg</v>
-      </c>
-      <c r="F28" t="s">
-        <v>402</v>
       </c>
       <c r="G28" t="str">
         <f>Users!J28</f>
@@ -6837,16 +6784,8 @@
         <f>Users!C29</f>
         <v>Juba</v>
       </c>
-      <c r="D29" t="str">
-        <f>Users!E29</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E29">
-        <f>Users!F29</f>
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>402</v>
+      <c r="D29" t="s">
+        <v>430</v>
       </c>
       <c r="G29" t="str">
         <f>Users!J29</f>
@@ -6870,16 +6809,12 @@
         <f>Users!C30</f>
         <v>Kang</v>
       </c>
-      <c r="D30" t="str">
-        <f>Users!E30</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D30" t="s">
+        <v>430</v>
       </c>
       <c r="E30" t="str">
         <f>Users!F30</f>
         <v>https://ist.rit.edu/assets/img/people/jwkics.jpg</v>
-      </c>
-      <c r="F30" t="s">
-        <v>402</v>
       </c>
       <c r="G30" t="str">
         <f>Users!J30</f>
@@ -6903,16 +6838,12 @@
         <f>Users!C31</f>
         <v>Kennedy</v>
       </c>
-      <c r="D31" t="str">
-        <f>Users!E31</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D31" t="s">
+        <v>430</v>
       </c>
       <c r="E31" t="str">
         <f>Users!F31</f>
         <v>https://ist.rit.edu/assets/img/people/drkisd.jpg</v>
-      </c>
-      <c r="F31" t="s">
-        <v>402</v>
       </c>
       <c r="G31" t="str">
         <f>Users!J31</f>
@@ -6936,16 +6867,8 @@
         <f>Users!C32</f>
         <v>Klossner</v>
       </c>
-      <c r="D32" t="str">
-        <f>Users!E32</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E32">
-        <f>Users!F32</f>
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>402</v>
+      <c r="D32" t="s">
+        <v>430</v>
       </c>
       <c r="G32" t="str">
         <f>Users!J32</f>
@@ -6969,16 +6892,8 @@
         <f>Users!C33</f>
         <v>Kuliner</v>
       </c>
-      <c r="D33" t="str">
-        <f>Users!E33</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E33">
-        <f>Users!F33</f>
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>402</v>
+      <c r="D33" t="s">
+        <v>430</v>
       </c>
       <c r="G33" t="str">
         <f>Users!J33</f>
@@ -7002,16 +6917,12 @@
         <f>Users!C34</f>
         <v>LaBelle</v>
       </c>
-      <c r="D34" t="str">
-        <f>Users!E34</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D34" t="s">
+        <v>430</v>
       </c>
       <c r="E34" t="str">
         <f>Users!F34</f>
         <v>https://ist.rit.edu/assets/img/people/dmlics.jpg</v>
-      </c>
-      <c r="F34" t="s">
-        <v>402</v>
       </c>
       <c r="G34" t="str">
         <f>Users!J34</f>
@@ -7035,16 +6946,12 @@
         <f>Users!C35</f>
         <v>Lasky</v>
       </c>
-      <c r="D35" t="str">
-        <f>Users!E35</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D35" t="s">
+        <v>430</v>
       </c>
       <c r="E35" t="str">
         <f>Users!F35</f>
         <v>https://ist.rit.edu/assets/img/people/jalics.jpg</v>
-      </c>
-      <c r="F35" t="s">
-        <v>402</v>
       </c>
       <c r="G35" t="str">
         <f>Users!J35</f>
@@ -7068,16 +6975,12 @@
         <f>Users!C36</f>
         <v>Leone</v>
       </c>
-      <c r="D36" t="str">
-        <f>Users!E36</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D36" t="s">
+        <v>430</v>
       </c>
       <c r="E36" t="str">
         <f>Users!F36</f>
         <v>https://ist.rit.edu/assets/img/people/jalvks.jpg</v>
-      </c>
-      <c r="F36" t="s">
-        <v>402</v>
       </c>
       <c r="G36" t="str">
         <f>Users!J36</f>
@@ -7101,16 +7004,8 @@
         <f>Users!C37</f>
         <v>Loporcaro</v>
       </c>
-      <c r="D37" t="str">
-        <f>Users!E37</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E37">
-        <f>Users!F37</f>
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>402</v>
+      <c r="D37" t="s">
+        <v>430</v>
       </c>
       <c r="G37" t="str">
         <f>Users!J37</f>
@@ -7134,16 +7029,12 @@
         <f>Users!C38</f>
         <v>Lutz</v>
       </c>
-      <c r="D38" t="str">
-        <f>Users!E38</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D38" t="s">
+        <v>430</v>
       </c>
       <c r="E38" t="str">
         <f>Users!F38</f>
         <v>https://ist.rit.edu/assets/img/people/phlics.jpg</v>
-      </c>
-      <c r="F38" t="s">
-        <v>402</v>
       </c>
       <c r="G38" t="str">
         <f>Users!J38</f>
@@ -7167,16 +7058,12 @@
         <f>Users!C39</f>
         <v>Mason</v>
       </c>
-      <c r="D39" t="str">
-        <f>Users!E39</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D39" t="s">
+        <v>430</v>
       </c>
       <c r="E39" t="str">
         <f>Users!F39</f>
         <v>https://ist.rit.edu/assets/img/people/spmics.jpg</v>
-      </c>
-      <c r="F39" t="s">
-        <v>402</v>
       </c>
       <c r="G39" t="str">
         <f>Users!J39</f>
@@ -7200,16 +7087,12 @@
         <f>Users!C40</f>
         <v>McQuaid</v>
       </c>
-      <c r="D40" t="str">
-        <f>Users!E40</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D40" t="s">
+        <v>430</v>
       </c>
       <c r="E40" t="str">
         <f>Users!F40</f>
         <v>https://ist.rit.edu/assets/img/people/mjmics.jpg</v>
-      </c>
-      <c r="F40" t="s">
-        <v>402</v>
       </c>
       <c r="G40" t="str">
         <f>Users!J40</f>
@@ -7233,16 +7116,12 @@
         <f>Users!C41</f>
         <v>Oh</v>
       </c>
-      <c r="D41" t="str">
-        <f>Users!E41</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D41" t="s">
+        <v>430</v>
       </c>
       <c r="E41" t="str">
         <f>Users!F41</f>
         <v>https://ist.rit.edu/assets/img/people/thoics.jpg</v>
-      </c>
-      <c r="F41" t="s">
-        <v>402</v>
       </c>
       <c r="G41" t="str">
         <f>Users!J41</f>
@@ -7266,16 +7145,12 @@
         <f>Users!C42</f>
         <v>Perez-Hardy</v>
       </c>
-      <c r="D42" t="str">
-        <f>Users!E42</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D42" t="s">
+        <v>430</v>
       </c>
       <c r="E42" t="str">
         <f>Users!F42</f>
         <v>https://ist.rit.edu/assets/img/people/sphics.jpg</v>
-      </c>
-      <c r="F42" t="s">
-        <v>402</v>
       </c>
       <c r="G42" t="str">
         <f>Users!J42</f>
@@ -7299,16 +7174,12 @@
         <f>Users!C43</f>
         <v>Powell</v>
       </c>
-      <c r="D43" t="str">
-        <f>Users!E43</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D43" t="s">
+        <v>430</v>
       </c>
       <c r="E43" t="str">
         <f>Users!F43</f>
         <v>https://ist.rit.edu/assets/img/people/djpihst.jpg</v>
-      </c>
-      <c r="F43" t="s">
-        <v>402</v>
       </c>
       <c r="G43" t="str">
         <f>Users!J43</f>
@@ -7332,16 +7203,8 @@
         <f>Users!C44</f>
         <v>Root II</v>
       </c>
-      <c r="D44" t="str">
-        <f>Users!E44</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E44">
-        <f>Users!F44</f>
-        <v>0</v>
-      </c>
-      <c r="F44" t="s">
-        <v>402</v>
+      <c r="D44" t="s">
+        <v>430</v>
       </c>
       <c r="G44" t="str">
         <f>Users!J44</f>
@@ -7365,16 +7228,8 @@
         <f>Users!C45</f>
         <v>Roth</v>
       </c>
-      <c r="D45" t="str">
-        <f>Users!E45</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E45">
-        <f>Users!F45</f>
-        <v>0</v>
-      </c>
-      <c r="F45" t="s">
-        <v>402</v>
+      <c r="D45" t="s">
+        <v>430</v>
       </c>
       <c r="G45" t="str">
         <f>Users!J45</f>
@@ -7398,16 +7253,8 @@
         <f>Users!C46</f>
         <v>Sabourin</v>
       </c>
-      <c r="D46" t="str">
-        <f>Users!E46</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E46">
-        <f>Users!F46</f>
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>402</v>
+      <c r="D46" t="s">
+        <v>430</v>
       </c>
       <c r="G46" t="str">
         <f>Users!J46</f>
@@ -7431,16 +7278,8 @@
         <f>Users!C47</f>
         <v>Schneider</v>
       </c>
-      <c r="D47" t="str">
-        <f>Users!E47</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E47">
-        <f>Users!F47</f>
-        <v>0</v>
-      </c>
-      <c r="F47" t="s">
-        <v>402</v>
+      <c r="D47" t="s">
+        <v>430</v>
       </c>
       <c r="G47" t="str">
         <f>Users!J47</f>
@@ -7464,16 +7303,12 @@
         <f>Users!C48</f>
         <v>Shenoy</v>
       </c>
-      <c r="D48" t="str">
-        <f>Users!E48</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D48" t="s">
+        <v>430</v>
       </c>
       <c r="E48" t="str">
         <f>Users!F48</f>
         <v>https://ist.rit.edu/assets/img/people/nxsvks.jpg</v>
-      </c>
-      <c r="F48" t="s">
-        <v>402</v>
       </c>
       <c r="G48" t="str">
         <f>Users!J48</f>
@@ -7497,16 +7332,12 @@
         <f>Users!C49</f>
         <v>Smith</v>
       </c>
-      <c r="D49" t="str">
-        <f>Users!E49</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D49" t="s">
+        <v>430</v>
       </c>
       <c r="E49" t="str">
         <f>Users!F49</f>
         <v>https://ist.rit.edu/assets/img/people/aesfaa.jpg</v>
-      </c>
-      <c r="F49" t="s">
-        <v>402</v>
       </c>
       <c r="G49" t="str">
         <f>Users!J49</f>
@@ -7530,16 +7361,8 @@
         <f>Users!C50</f>
         <v>Takats</v>
       </c>
-      <c r="D50" t="str">
-        <f>Users!E50</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
-      </c>
-      <c r="E50">
-        <f>Users!F50</f>
-        <v>0</v>
-      </c>
-      <c r="F50" t="s">
-        <v>402</v>
+      <c r="D50" t="s">
+        <v>430</v>
       </c>
       <c r="G50" t="str">
         <f>Users!J50</f>
@@ -7563,16 +7386,12 @@
         <f>Users!C51</f>
         <v>Tomaszewski</v>
       </c>
-      <c r="D51" t="str">
-        <f>Users!E51</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D51" t="s">
+        <v>430</v>
       </c>
       <c r="E51" t="str">
         <f>Users!F51</f>
         <v>https://ist.rit.edu/assets/img/people/bmtski.jpg</v>
-      </c>
-      <c r="F51" t="s">
-        <v>402</v>
       </c>
       <c r="G51" t="str">
         <f>Users!J51</f>
@@ -7596,16 +7415,12 @@
         <f>Users!C52</f>
         <v>Vullo</v>
       </c>
-      <c r="D52" t="str">
-        <f>Users!E52</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D52" t="s">
+        <v>430</v>
       </c>
       <c r="E52" t="str">
         <f>Users!F52</f>
         <v>https://ist.rit.edu/assets/img/people/rpvvks.jpg</v>
-      </c>
-      <c r="F52" t="s">
-        <v>402</v>
       </c>
       <c r="G52" t="str">
         <f>Users!J52</f>
@@ -7629,16 +7444,12 @@
         <f>Users!C53</f>
         <v>Warren</v>
       </c>
-      <c r="D53" t="str">
-        <f>Users!E53</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D53" t="s">
+        <v>430</v>
       </c>
       <c r="E53" t="str">
         <f>Users!F53</f>
         <v>https://www.rit.edu/gccis/sites/rit.edu.gccis/files//ann.jpg</v>
-      </c>
-      <c r="F53" t="s">
-        <v>402</v>
       </c>
       <c r="G53" t="str">
         <f>Users!J53</f>
@@ -7662,16 +7473,12 @@
         <f>Users!C54</f>
         <v>Weeden</v>
       </c>
-      <c r="D54" t="str">
-        <f>Users!E54</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D54" t="s">
+        <v>430</v>
       </c>
       <c r="E54" t="str">
         <f>Users!F54</f>
         <v>https://ist.rit.edu/assets/img/people/emwics.jpg</v>
-      </c>
-      <c r="F54" t="s">
-        <v>402</v>
       </c>
       <c r="G54" t="str">
         <f>Users!J54</f>
@@ -7695,16 +7502,12 @@
         <f>Users!C55</f>
         <v>Weissman</v>
       </c>
-      <c r="D55" t="str">
-        <f>Users!E55</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D55" t="s">
+        <v>430</v>
       </c>
       <c r="E55" t="str">
         <f>Users!F55</f>
         <v>https://www.rit.edu/gccis/sites/rit.edu.gccis/files//jweissman%5B1%5D.jpg</v>
-      </c>
-      <c r="F55" t="s">
-        <v>402</v>
       </c>
       <c r="G55" t="str">
         <f>Users!J55</f>
@@ -7728,16 +7531,12 @@
         <f>Users!C56</f>
         <v>Yacci</v>
       </c>
-      <c r="D56" t="str">
-        <f>Users!E56</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D56" t="s">
+        <v>430</v>
       </c>
       <c r="E56" t="str">
         <f>Users!F56</f>
         <v>https://www.rit.edu/gccis//sites/rit.edu.gccis/files//yacci%20new%20headshot.jpg</v>
-      </c>
-      <c r="F56" t="s">
-        <v>402</v>
       </c>
       <c r="G56" t="str">
         <f>Users!J56</f>
@@ -7761,16 +7560,12 @@
         <f>Users!C57</f>
         <v>Yu</v>
       </c>
-      <c r="D57" t="str">
-        <f>Users!E57</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D57" t="s">
+        <v>430</v>
       </c>
       <c r="E57" t="str">
         <f>Users!F57</f>
         <v>https://ist.rit.edu/assets/img/people/qyuvks.jpg</v>
-      </c>
-      <c r="F57" t="s">
-        <v>402</v>
       </c>
       <c r="G57" t="str">
         <f>Users!J57</f>
@@ -7794,16 +7589,12 @@
         <f>Users!C58</f>
         <v>Zilora</v>
       </c>
-      <c r="D58" t="str">
-        <f>Users!E58</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D58" t="s">
+        <v>430</v>
       </c>
       <c r="E58" t="str">
         <f>Users!F58</f>
         <v>https://ist.rit.edu/assets/img/people/sjzics.jpg</v>
-      </c>
-      <c r="F58" t="s">
-        <v>402</v>
       </c>
       <c r="G58" t="str">
         <f>Users!J58</f>
@@ -7827,16 +7618,12 @@
         <f>Users!C59</f>
         <v>Baker-Smith</v>
       </c>
-      <c r="D59" t="str">
-        <f>Users!E59</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D59" t="s">
+        <v>430</v>
       </c>
       <c r="E59" t="str">
         <f>Users!F59</f>
         <v>https://ist.rit.edu/assets/img/people/rdbcst.jpg</v>
-      </c>
-      <c r="F59" t="s">
-        <v>402</v>
       </c>
       <c r="G59" t="str">
         <f>Users!J59</f>
@@ -7860,16 +7647,12 @@
         <f>Users!C60</f>
         <v>Yu</v>
       </c>
-      <c r="D60" t="str">
-        <f>Users!E60</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D60" t="s">
+        <v>430</v>
       </c>
       <c r="E60" t="str">
         <f>Users!F60</f>
         <v>https://ist.rit.edu/assets/img/people/qyuvks.jpg</v>
-      </c>
-      <c r="F60" t="s">
-        <v>402</v>
       </c>
       <c r="G60" t="str">
         <f>Users!J60</f>
@@ -7893,16 +7676,12 @@
         <f>Users!C61</f>
         <v>Hanna</v>
       </c>
-      <c r="D61" t="str">
-        <f>Users!E61</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D61" t="s">
+        <v>430</v>
       </c>
       <c r="E61" t="str">
         <f>Users!F61</f>
         <v>https://ist.rit.edu/assets/img/people/mchics.jpg</v>
-      </c>
-      <c r="F61" t="s">
-        <v>402</v>
       </c>
       <c r="G61" t="str">
         <f>Users!J61</f>
@@ -7926,16 +7705,12 @@
         <f>Users!C62</f>
         <v>Persson</v>
       </c>
-      <c r="D62" t="str">
-        <f>Users!E62</f>
-        <v>5f4dcc3b5aa765d61d8327deb882cf99</v>
+      <c r="D62" t="s">
+        <v>430</v>
       </c>
       <c r="E62" t="str">
         <f>Users!F62</f>
         <v>https://ist.rit.edu/assets/img/people/jmpics.jpg</v>
-      </c>
-      <c r="F62" t="s">
-        <v>402</v>
       </c>
       <c r="G62" t="str">
         <f>Users!J62</f>

</xml_diff>